<commit_message>
ADEDD COMPUTATION OF LEAF SUN AND SHADE CARBON AND THEIR RELATIVE MAINTEINANCE RESPIRATION
</commit_message>
<xml_diff>
--- a/software/3D-CMCC-Forest-Model/tables/CO2_mod_assimilation.xlsx
+++ b/software/3D-CMCC-Forest-Model/tables/CO2_mod_assimilation.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="9270" windowHeight="3615" tabRatio="754" firstSheet="6" activeTab="16"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="9270" windowHeight="3615" tabRatio="754" firstSheet="6" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Fco2 8.5" sheetId="1" r:id="rId1"/>
@@ -244,7 +244,7 @@
     <t>fCO2 * fT (RCP 8.5)</t>
   </si>
   <si>
-    <t>fCO2 * fT (HistRep)</t>
+    <t>fCO2 * fT (Control)</t>
   </si>
 </sst>
 </file>
@@ -1343,25 +1343,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="113489408"/>
-        <c:axId val="113490944"/>
+        <c:axId val="127838464"/>
+        <c:axId val="128149376"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="113489408"/>
+        <c:axId val="127838464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113490944"/>
+        <c:crossAx val="128149376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="113490944"/>
+        <c:axId val="128149376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1369,7 +1369,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113489408"/>
+        <c:crossAx val="127838464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1381,7 +1381,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1420,7 +1420,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="-8.3873140857392864E-2"/>
-                  <c:y val="0.48100685331000337"/>
+                  <c:y val="0.48100685331000342"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1595,7 +1595,7 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-8.1095363079615221E-2"/>
+                  <c:x val="-8.1095363079615235E-2"/>
                   <c:y val="0.3450182268883058"/>
                 </c:manualLayout>
               </c:layout>
@@ -1771,8 +1771,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-8.1095363079615221E-2"/>
-                  <c:y val="0.32103127734033271"/>
+                  <c:x val="-8.1095363079615235E-2"/>
+                  <c:y val="0.32103127734033277"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1948,7 +1948,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="-9.1428696412948332E-2"/>
-                  <c:y val="0.28656022163896205"/>
+                  <c:y val="0.28656022163896211"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -2100,24 +2100,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="58518912"/>
-        <c:axId val="58520704"/>
+        <c:axId val="138813440"/>
+        <c:axId val="138814976"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="58518912"/>
+        <c:axId val="138813440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58520704"/>
+        <c:crossAx val="138814976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="58520704"/>
+        <c:axId val="138814976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2125,7 +2125,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58518912"/>
+        <c:crossAx val="138813440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2138,7 +2138,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2157,7 +2157,7 @@
           <c:x val="0.11290507436570428"/>
           <c:y val="5.1400554097404488E-2"/>
           <c:w val="0.53881671041119861"/>
-          <c:h val="0.81873067949839673"/>
+          <c:h val="0.81873067949839684"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -2392,7 +2392,7 @@
               <c:idx val="19"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-1.6666666666666677E-2"/>
+                  <c:x val="-1.666666666666668E-2"/>
                   <c:y val="-5.0925925925925923E-2"/>
                 </c:manualLayout>
               </c:layout>
@@ -2582,8 +2582,8 @@
               <c:idx val="19"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-3.6111111111111129E-2"/>
-                  <c:y val="-3.2407407407407426E-2"/>
+                  <c:x val="-3.6111111111111135E-2"/>
+                  <c:y val="-3.2407407407407433E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -2772,8 +2772,8 @@
               <c:idx val="18"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-3.6111111111111129E-2"/>
-                  <c:y val="-2.7777777777777853E-2"/>
+                  <c:x val="-3.6111111111111135E-2"/>
+                  <c:y val="-2.7777777777777863E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -2923,8 +2923,8 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="140760960"/>
-        <c:axId val="140652544"/>
+        <c:axId val="138963200"/>
+        <c:axId val="138969472"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -2937,7 +2937,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>fCO2 * fT (HistRep)</c:v>
+                  <c:v>fCO2 * fT (Control)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2968,8 +2968,8 @@
               <c:idx val="19"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-5.5555555555555518E-2"/>
-                  <c:y val="2.7777777777777811E-2"/>
+                  <c:x val="-5.5555555555555504E-2"/>
+                  <c:y val="2.7777777777777821E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -3268,11 +3268,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="140656000"/>
-        <c:axId val="140654464"/>
+        <c:axId val="138985472"/>
+        <c:axId val="138971392"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="140760960"/>
+        <c:axId val="138963200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3323,7 +3323,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="140652544"/>
+        <c:crossAx val="138969472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3332,7 +3332,7 @@
         <c:tickMarkSkip val="5"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="140652544"/>
+        <c:axId val="138969472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3384,7 +3384,7 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="2.7777777777777822E-3"/>
+              <c:x val="2.7777777777777835E-3"/>
               <c:y val="0.36409922717993587"/>
             </c:manualLayout>
           </c:layout>
@@ -3412,13 +3412,13 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="140760960"/>
+        <c:crossAx val="138963200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="0.30000000000000021"/>
+        <c:majorUnit val="0.30000000000000027"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="140654464"/>
+        <c:axId val="138971392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2.1"/>
@@ -3434,13 +3434,13 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="140656000"/>
+        <c:crossAx val="138985472"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="0.30000000000000021"/>
+        <c:majorUnit val="0.30000000000000027"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="140656000"/>
+        <c:axId val="138985472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3455,7 +3455,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="140654464"/>
+        <c:crossAx val="138971392"/>
         <c:crosses val="max"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3490,7 +3490,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
@@ -7257,31 +7257,31 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="113605632"/>
-        <c:axId val="113612672"/>
+        <c:axId val="128063360"/>
+        <c:axId val="128064896"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="113605632"/>
+        <c:axId val="128063360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113612672"/>
+        <c:crossAx val="128064896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="113612672"/>
+        <c:axId val="128064896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113605632"/>
+        <c:crossAx val="128063360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7294,7 +7294,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7311,10 +7311,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.13903807068672272"/>
-          <c:y val="9.2951662292213577E-2"/>
+          <c:x val="0.13903807068672275"/>
+          <c:y val="9.2951662292213591E-2"/>
           <c:w val="0.80905891213466563"/>
-          <c:h val="0.7490547535724712"/>
+          <c:h val="0.74905475357247142"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -9321,8 +9321,8 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="115931008"/>
-        <c:axId val="116806784"/>
+        <c:axId val="138067328"/>
+        <c:axId val="138077696"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -9994,11 +9994,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="118151808"/>
-        <c:axId val="118149888"/>
+        <c:axId val="137958528"/>
+        <c:axId val="138079616"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="115931008"/>
+        <c:axId val="138067328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10050,7 +10050,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="116806784"/>
+        <c:crossAx val="138077696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10059,7 +10059,7 @@
         <c:tickMarkSkip val="10"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="116806784"/>
+        <c:axId val="138077696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2.6"/>
@@ -10106,7 +10106,7 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="1.9907842530435425E-3"/>
+              <c:x val="1.9907842530435429E-3"/>
               <c:y val="0.35421515018955962"/>
             </c:manualLayout>
           </c:layout>
@@ -10134,13 +10134,13 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="115931008"/>
+        <c:crossAx val="138067328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.30000000000000032"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="118149888"/>
+        <c:axId val="138079616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2.6"/>
@@ -10157,13 +10157,13 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="118151808"/>
+        <c:crossAx val="137958528"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="0.30000000000000027"/>
+        <c:majorUnit val="0.30000000000000032"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="118151808"/>
+        <c:axId val="137958528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10178,7 +10178,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="118149888"/>
+        <c:crossAx val="138079616"/>
         <c:crosses val="max"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10196,7 +10196,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
@@ -10214,10 +10214,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.11846062992126009"/>
+          <c:x val="0.11846062992126011"/>
           <c:y val="0.12535906969962088"/>
-          <c:w val="0.60677974628171583"/>
-          <c:h val="0.75866105278506923"/>
+          <c:w val="0.60677974628171594"/>
+          <c:h val="0.75866105278506935"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -12230,8 +12230,8 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="110790144"/>
-        <c:axId val="110791680"/>
+        <c:axId val="138000256"/>
+        <c:axId val="138001792"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -12905,11 +12905,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="110807680"/>
-        <c:axId val="110806144"/>
+        <c:axId val="138013696"/>
+        <c:axId val="138012160"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="110790144"/>
+        <c:axId val="138000256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12923,7 +12923,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="110791680"/>
+        <c:crossAx val="138001792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12932,7 +12932,7 @@
         <c:tickMarkSkip val="10"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="110791680"/>
+        <c:axId val="138001792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.30000000000000032"/>
@@ -12959,7 +12959,7 @@
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
               <c:x val="8.3333333333333367E-3"/>
-              <c:y val="0.37967811315252314"/>
+              <c:y val="0.37967811315252326"/>
             </c:manualLayout>
           </c:layout>
         </c:title>
@@ -12973,17 +12973,17 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="110790144"/>
+        <c:crossAx val="138000256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="110806144"/>
+        <c:axId val="138012160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.1000000000000001"/>
-          <c:min val="0.30000000000000016"/>
+          <c:min val="0.30000000000000021"/>
         </c:scaling>
         <c:axPos val="r"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -12996,13 +12996,13 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="110807680"/>
+        <c:crossAx val="138013696"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="110807680"/>
+        <c:axId val="138013696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13016,7 +13016,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="110806144"/>
+        <c:crossAx val="138012160"/>
         <c:crosses val="max"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13038,7 +13038,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000002" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000002" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -13055,9 +13055,9 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.14093373881701754"/>
+          <c:x val="0.14093373881701757"/>
           <c:y val="9.7581291921843102E-2"/>
-          <c:w val="0.82491937448854868"/>
+          <c:w val="0.8249193744885488"/>
           <c:h val="0.74477216389617962"/>
         </c:manualLayout>
       </c:layout>
@@ -14030,8 +14030,8 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="140117120"/>
-        <c:axId val="140119040"/>
+        <c:axId val="138155520"/>
+        <c:axId val="138157440"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -14358,11 +14358,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="140130944"/>
-        <c:axId val="140129408"/>
+        <c:axId val="138169344"/>
+        <c:axId val="138167808"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="140117120"/>
+        <c:axId val="138155520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14414,7 +14414,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="140119040"/>
+        <c:crossAx val="138157440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14423,7 +14423,7 @@
         <c:tickMarkSkip val="5"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="140119040"/>
+        <c:axId val="138157440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2.6"/>
@@ -14470,8 +14470,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="2.7969730144960302E-3"/>
-              <c:y val="0.35207385535141461"/>
+              <c:x val="2.7969730144960306E-3"/>
+              <c:y val="0.35207385535141467"/>
             </c:manualLayout>
           </c:layout>
         </c:title>
@@ -14498,13 +14498,13 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="140117120"/>
+        <c:crossAx val="138155520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="0.30000000000000027"/>
+        <c:majorUnit val="0.30000000000000032"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="140129408"/>
+        <c:axId val="138167808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2.6"/>
@@ -14521,13 +14521,13 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="140130944"/>
+        <c:crossAx val="138169344"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="0.30000000000000027"/>
+        <c:majorUnit val="0.30000000000000032"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="140130944"/>
+        <c:axId val="138169344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14542,7 +14542,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="140129408"/>
+        <c:crossAx val="138167808"/>
         <c:crosses val="max"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14560,7 +14560,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
@@ -16484,24 +16484,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="140148096"/>
-        <c:axId val="140162176"/>
+        <c:axId val="138207232"/>
+        <c:axId val="138208768"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="140148096"/>
+        <c:axId val="138207232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="140162176"/>
+        <c:crossAx val="138208768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="140162176"/>
+        <c:axId val="138208768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16509,19 +16509,20 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="140148096"/>
+        <c:crossAx val="138207232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -16531,7 +16532,9 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="it-IT"/>
   <c:chart>
-    <c:title/>
+    <c:title>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -16699,24 +16702,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="140285056"/>
-        <c:axId val="140286592"/>
+        <c:axId val="138372608"/>
+        <c:axId val="138374144"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="140285056"/>
+        <c:axId val="138372608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="140286592"/>
+        <c:crossAx val="138374144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="140286592"/>
+        <c:axId val="138374144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16724,19 +16727,20 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="140285056"/>
+        <c:crossAx val="138372608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -16767,6 +16771,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout>
@@ -16777,7 +16782,7 @@
           <c:x val="0.13885825799675508"/>
           <c:y val="0.19480351414406533"/>
           <c:w val="0.55041367671352592"/>
-          <c:h val="0.68921660834062393"/>
+          <c:h val="0.68921660834062382"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -18075,11 +18080,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="140448512"/>
-        <c:axId val="140450048"/>
+        <c:axId val="138286208"/>
+        <c:axId val="138287744"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="140448512"/>
+        <c:axId val="138286208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18097,7 +18102,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="140450048"/>
+        <c:crossAx val="138287744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -18106,7 +18111,7 @@
         <c:tickMarkSkip val="5"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="140450048"/>
+        <c:axId val="138287744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.5"/>
@@ -18128,11 +18133,12 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="140448512"/>
+        <c:crossAx val="138286208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -18143,10 +18149,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.63823951030508375"/>
+          <c:x val="0.63823951030508386"/>
           <c:y val="2.3869568387284931E-2"/>
-          <c:w val="0.34497865160794083"/>
-          <c:h val="0.6697375328084002"/>
+          <c:w val="0.34497865160794094"/>
+          <c:h val="0.66973753280840043"/>
         </c:manualLayout>
       </c:layout>
     </c:legend>
@@ -18159,7 +18165,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -18200,7 +18206,7 @@
                   <c:v>9.2365704660169107E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.18064128360710077</c:v>
+                  <c:v>0.18064128360710083</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.26478007357174982</c:v>
@@ -18209,19 +18215,19 @@
                   <c:v>0.3447329706020868</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.42044820762685764</c:v>
+                  <c:v>0.42044820762685775</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.49187110296247866</c:v>
+                  <c:v>0.49187110296247877</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.55894377476921331</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.62160481538672518</c:v>
+                  <c:v>0.62160481538672541</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.67978891812111675</c:v>
+                  <c:v>0.67978891812111686</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0.7334264473278278</c:v>
@@ -18239,7 +18245,7 @@
                   <c:v>0.90093626092041956</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.93060485910210022</c:v>
+                  <c:v>0.93060485910210033</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>0.9551833496505987</c:v>
@@ -18248,7 +18254,7 @@
                   <c:v>0.97455164804845462</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.98857757847701733</c:v>
+                  <c:v>0.98857757847701722</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>0.99711476677448452</c:v>
@@ -18260,25 +18266,25 @@
                   <c:v>0.99704987076304064</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.98805644438066209</c:v>
+                  <c:v>0.98805644438066198</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.97278156236531943</c:v>
+                  <c:v>0.97278156236531954</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.95094919608674455</c:v>
+                  <c:v>0.95094919608674466</c:v>
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>0.9222349330836016</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.88625110584464895</c:v>
+                  <c:v>0.88625110584464872</c:v>
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>0.84252503495545772</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.79046586688263332</c:v>
+                  <c:v>0.79046586688263321</c:v>
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>0.7293113892161025</c:v>
@@ -18290,10 +18296,10 @@
                   <c:v>0.57518592130083979</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.47851160999079101</c:v>
+                  <c:v>0.47851160999079106</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.36407260116115647</c:v>
+                  <c:v>0.36407260116115653</c:v>
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>0.2230388294100821</c:v>
@@ -18359,13 +18365,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="45"/>
                 <c:pt idx="0">
-                  <c:v>0.10021417393114176</c:v>
+                  <c:v>0.10021417393114178</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.19853073939348898</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.29526175539994948</c:v>
+                  <c:v>0.29526175539994953</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.39073661752750588</c:v>
@@ -18383,13 +18389,13 @@
                   <c:v>0.7665795583972147</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.86037268582620741</c:v>
+                  <c:v>0.8603726858262073</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0.95438753848767544</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.0485613487076619</c:v>
+                  <c:v>1.0485613487076617</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>1.1426634088476042</c:v>
@@ -18404,7 +18410,7 @@
                   <c:v>1.5649442729917202</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.633764083147291</c:v>
+                  <c:v>1.6337640831472908</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>1.6949090104485021</c:v>
@@ -18416,10 +18422,10 @@
                   <c:v>1.7910660009078778</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.8244216837340668</c:v>
+                  <c:v>1.8244216837340665</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.8467855424463688</c:v>
+                  <c:v>1.8467855424463691</c:v>
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>1.8572139287081761</c:v>
@@ -18440,10 +18446,10 @@
                   <c:v>1.6921838181920101</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1.60642306259747</c:v>
+                  <c:v>1.6064230625974698</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1.498946713099969</c:v>
+                  <c:v>1.4989467130999687</c:v>
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>1.3671185906124033</c:v>
@@ -18455,7 +18461,7 @@
                   <c:v>1.0143435175638187</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.77900961120782308</c:v>
+                  <c:v>0.7790096112078233</c:v>
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>0.48150412064779452</c:v>
@@ -18521,7 +18527,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="45"/>
                 <c:pt idx="0">
-                  <c:v>9.8062466940922757E-2</c:v>
+                  <c:v>9.8062466940922785E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.19358025964333125</c:v>
@@ -18530,10 +18536,10 @@
                   <c:v>0.28673773311675776</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.37772036567652056</c:v>
+                  <c:v>0.37772036567652062</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.46670502458363178</c:v>
+                  <c:v>0.46670502458363172</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.55384761090795187</c:v>
@@ -18545,13 +18551,13 @@
                   <c:v>0.72303410068956275</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.80514166947809296</c:v>
+                  <c:v>0.80514166947809318</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0.88549805143579763</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.96390445481151343</c:v>
+                  <c:v>0.96390445481151354</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>1.0400427182385021</c:v>
@@ -18566,10 +18572,10 @@
                   <c:v>1.3307120811781841</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.3805080368752563</c:v>
+                  <c:v>1.3805080368752565</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.4232466809113082</c:v>
+                  <c:v>1.423246680911308</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>1.4584460870262779</c:v>
@@ -18578,7 +18584,7 @@
                   <c:v>1.4856036209110217</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.5041937046837108</c:v>
+                  <c:v>1.5041937046837111</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>1.5136641044658432</c:v>
@@ -18590,34 +18596,34 @@
                   <c:v>1.5028670149269521</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.4812966379613846</c:v>
+                  <c:v>1.4812966379613843</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.4479717533072201</c:v>
+                  <c:v>1.4479717533072196</c:v>
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>1.4020504863255789</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1.3425596608469239</c:v>
+                  <c:v>1.3425596608469241</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1.2683383820393328</c:v>
+                  <c:v>1.2683383820393326</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1.1779474620235439</c:v>
+                  <c:v>1.1779474620235442</c:v>
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>1.0695146229515704</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.94044642771036868</c:v>
+                  <c:v>0.94044642771036857</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.78682353916319625</c:v>
+                  <c:v>0.78682353916319636</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.60187400597340979</c:v>
+                  <c:v>0.6018740059734099</c:v>
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>0.37060283264538046</c:v>
@@ -18689,10 +18695,10 @@
                   <c:v>0.18955765602267871</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.27986186582092665</c:v>
+                  <c:v>0.27986186582092676</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.36730731947426015</c:v>
+                  <c:v>0.36730731947426026</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.45197312127122591</c:v>
@@ -18716,7 +18722,7 @@
                   <c:v>0.90193334012542559</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.96619646915857571</c:v>
+                  <c:v>0.96619646915857582</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>1.0266773191772665</c:v>
@@ -18737,7 +18743,7 @@
                   <c:v>1.2784248291881255</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.2973097417744084</c:v>
+                  <c:v>1.2973097417744082</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>1.3087047947928518</c:v>
@@ -18749,19 +18755,19 @@
                   <c:v>1.3074626349784766</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.2939677051574874</c:v>
+                  <c:v>1.2939677051574872</c:v>
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>1.2712494161600338</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.2387554945563437</c:v>
+                  <c:v>1.2387554945563439</c:v>
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>1.1958524050073249</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1.1417945500900533</c:v>
+                  <c:v>1.141794550090053</c:v>
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>1.075677317835859</c:v>
@@ -18776,13 +18782,13 @@
                   <c:v>0.791529350007671</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.66070267765119073</c:v>
+                  <c:v>0.66070267765119095</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.50428790170812499</c:v>
+                  <c:v>0.50428790170812487</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.30986544460407117</c:v>
+                  <c:v>0.30986544460407123</c:v>
                 </c:pt>
                 <c:pt idx="34">
                   <c:v>0</c:v>
@@ -18845,19 +18851,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="45"/>
                 <c:pt idx="0">
-                  <c:v>9.3888750592002732E-2</c:v>
+                  <c:v>9.3888750592002745E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.18407696146349506</c:v>
+                  <c:v>0.18407696146349509</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.270565668816864</c:v>
+                  <c:v>0.27056566881686406</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.35334998576091337</c:v>
+                  <c:v>0.35334998576091342</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.43241586213369743</c:v>
+                  <c:v>0.43241586213369754</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.50773644019627351</c:v>
@@ -18866,7 +18872,7 @@
                   <c:v>0.57926820452287275</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.64694720625591307</c:v>
+                  <c:v>0.64694720625591329</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.71068570411516863</c:v>
@@ -18881,16 +18887,16 @@
                   <c:v>0.87697777903432705</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.92353564319318204</c:v>
+                  <c:v>0.92353564319318215</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0.96530990740761735</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.0158985246562515</c:v>
+                  <c:v>1.0158985246562517</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.0450940058400759</c:v>
+                  <c:v>1.0450940058400757</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>1.0686259386672061</c:v>
@@ -18905,7 +18911,7 @@
                   <c:v>1.1032635577033438</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.1020827360887024</c:v>
+                  <c:v>1.1020827360887029</c:v>
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>1.094114306579181</c:v>
@@ -18914,10 +18920,10 @@
                   <c:v>1.0790599793926641</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.0565811891463437</c:v>
+                  <c:v>1.0565811891463439</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.0262871543323424</c:v>
+                  <c:v>1.0262871543323426</c:v>
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>0.98771798007788858</c:v>
@@ -18932,10 +18938,10 @@
                   <c:v>0.81610515885680768</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.73724019230546023</c:v>
+                  <c:v>0.73724019230546034</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.64515513122280954</c:v>
+                  <c:v>0.64515513122280965</c:v>
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>0.53730188735690854</c:v>
@@ -18984,11 +18990,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="140638848"/>
-        <c:axId val="58471168"/>
+        <c:axId val="138742784"/>
+        <c:axId val="138753152"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="140638848"/>
+        <c:axId val="138742784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19013,7 +19019,7 @@
         </c:title>
         <c:majorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58471168"/>
+        <c:crossAx val="138753152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -19022,7 +19028,7 @@
         <c:tickMarkSkip val="3"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="58471168"/>
+        <c:axId val="138753152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19048,7 +19054,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="140638848"/>
+        <c:crossAx val="138742784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -19061,7 +19067,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -38891,8 +38897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Y9" sqref="Y9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -57214,7 +57220,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M151"/>
   <sheetViews>
-    <sheetView topLeftCell="J7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="J7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="AD8" sqref="AD8"/>
     </sheetView>
   </sheetViews>

</xml_diff>